<commit_message>
update clinical prodrome spreadsheet with data from pdfs retrieved 26/06
</commit_message>
<xml_diff>
--- a/Research/Prodrome/Prodrome EEG summary.xlsx
+++ b/Research/Prodrome/Prodrome EEG summary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvasey/Desktop/Besag/FB/Prodrome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvasey/Desktop/Besag/Research/Prodrome/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="660" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EEG Summaries" sheetId="1" r:id="rId1"/>
@@ -3671,33 +3671,207 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="149" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="150" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="72" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="78" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3716,179 +3890,101 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="117" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="118" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="153" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="152" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="154" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="72" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="78" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="116" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="146" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3945,102 +4041,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="142" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="117" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="118" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="116" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="153" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="152" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="154" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4336,7 +4336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AV110"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4355,451 +4355,451 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:48" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K2" s="166" t="s">
+      <c r="K2" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="L2" s="166"/>
-      <c r="M2" s="166"/>
-      <c r="N2" s="166"/>
-      <c r="O2" s="166"/>
-      <c r="P2" s="166"/>
-      <c r="Q2" s="166"/>
-      <c r="R2" s="166"/>
-      <c r="S2" s="166"/>
-      <c r="T2" s="166"/>
-      <c r="U2" s="166"/>
-      <c r="V2" s="167"/>
-      <c r="W2" s="168" t="s">
+      <c r="L2" s="165"/>
+      <c r="M2" s="165"/>
+      <c r="N2" s="165"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
+      <c r="S2" s="165"/>
+      <c r="T2" s="165"/>
+      <c r="U2" s="165"/>
+      <c r="V2" s="166"/>
+      <c r="W2" s="167" t="s">
         <v>127</v>
       </c>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="168"/>
-      <c r="Z2" s="168"/>
-      <c r="AA2" s="168"/>
-      <c r="AB2" s="168"/>
-      <c r="AC2" s="168"/>
-      <c r="AD2" s="168"/>
-      <c r="AE2" s="168"/>
-      <c r="AF2" s="168"/>
-      <c r="AG2" s="168"/>
-      <c r="AH2" s="169"/>
-      <c r="AI2" s="148" t="s">
+      <c r="X2" s="167"/>
+      <c r="Y2" s="167"/>
+      <c r="Z2" s="167"/>
+      <c r="AA2" s="167"/>
+      <c r="AB2" s="167"/>
+      <c r="AC2" s="167"/>
+      <c r="AD2" s="167"/>
+      <c r="AE2" s="167"/>
+      <c r="AF2" s="167"/>
+      <c r="AG2" s="167"/>
+      <c r="AH2" s="168"/>
+      <c r="AI2" s="206" t="s">
         <v>145</v>
       </c>
-      <c r="AJ2" s="148"/>
-      <c r="AK2" s="148"/>
-      <c r="AL2" s="148"/>
-      <c r="AM2" s="148"/>
-      <c r="AN2" s="148"/>
-      <c r="AO2" s="148"/>
-      <c r="AP2" s="148"/>
-      <c r="AQ2" s="148"/>
-      <c r="AR2" s="148"/>
-      <c r="AS2" s="148"/>
-      <c r="AT2" s="148"/>
-      <c r="AU2" s="149"/>
-      <c r="AV2" s="145"/>
+      <c r="AJ2" s="206"/>
+      <c r="AK2" s="206"/>
+      <c r="AL2" s="206"/>
+      <c r="AM2" s="206"/>
+      <c r="AN2" s="206"/>
+      <c r="AO2" s="206"/>
+      <c r="AP2" s="206"/>
+      <c r="AQ2" s="206"/>
+      <c r="AR2" s="206"/>
+      <c r="AS2" s="206"/>
+      <c r="AT2" s="206"/>
+      <c r="AU2" s="207"/>
+      <c r="AV2" s="205"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
-      <c r="B3" s="141"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="185" t="s">
+      <c r="B3" s="149"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="203"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="204"/>
+      <c r="K3" s="150" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="185"/>
-      <c r="M3" s="185"/>
-      <c r="N3" s="185"/>
-      <c r="O3" s="185"/>
-      <c r="P3" s="185"/>
-      <c r="Q3" s="185"/>
-      <c r="R3" s="185"/>
-      <c r="S3" s="208"/>
-      <c r="T3" s="184" t="s">
+      <c r="L3" s="150"/>
+      <c r="M3" s="150"/>
+      <c r="N3" s="150"/>
+      <c r="O3" s="150"/>
+      <c r="P3" s="150"/>
+      <c r="Q3" s="150"/>
+      <c r="R3" s="150"/>
+      <c r="S3" s="151"/>
+      <c r="T3" s="185" t="s">
         <v>126</v>
       </c>
-      <c r="U3" s="185"/>
+      <c r="U3" s="150"/>
       <c r="V3" s="186"/>
-      <c r="W3" s="180" t="s">
+      <c r="W3" s="181" t="s">
         <v>131</v>
       </c>
-      <c r="X3" s="180"/>
-      <c r="Y3" s="181"/>
-      <c r="Z3" s="182" t="s">
+      <c r="X3" s="181"/>
+      <c r="Y3" s="182"/>
+      <c r="Z3" s="183" t="s">
         <v>132</v>
       </c>
-      <c r="AA3" s="180"/>
-      <c r="AB3" s="180"/>
-      <c r="AC3" s="180"/>
-      <c r="AD3" s="180"/>
-      <c r="AE3" s="183"/>
-      <c r="AF3" s="181"/>
-      <c r="AG3" s="170"/>
-      <c r="AH3" s="171"/>
-      <c r="AI3" s="162" t="s">
+      <c r="AA3" s="181"/>
+      <c r="AB3" s="181"/>
+      <c r="AC3" s="181"/>
+      <c r="AD3" s="181"/>
+      <c r="AE3" s="184"/>
+      <c r="AF3" s="182"/>
+      <c r="AG3" s="169"/>
+      <c r="AH3" s="170"/>
+      <c r="AI3" s="195" t="s">
         <v>140</v>
       </c>
-      <c r="AJ3" s="163"/>
-      <c r="AK3" s="164" t="s">
+      <c r="AJ3" s="196"/>
+      <c r="AK3" s="199" t="s">
         <v>141</v>
       </c>
-      <c r="AL3" s="162"/>
-      <c r="AM3" s="162"/>
-      <c r="AN3" s="162"/>
-      <c r="AO3" s="162"/>
-      <c r="AP3" s="162"/>
-      <c r="AQ3" s="162"/>
-      <c r="AR3" s="162"/>
-      <c r="AS3" s="165"/>
-      <c r="AT3" s="150" t="s">
+      <c r="AL3" s="195"/>
+      <c r="AM3" s="195"/>
+      <c r="AN3" s="195"/>
+      <c r="AO3" s="195"/>
+      <c r="AP3" s="195"/>
+      <c r="AQ3" s="195"/>
+      <c r="AR3" s="195"/>
+      <c r="AS3" s="200"/>
+      <c r="AT3" s="208" t="s">
         <v>180</v>
       </c>
-      <c r="AU3" s="151"/>
-      <c r="AV3" s="145"/>
+      <c r="AU3" s="209"/>
+      <c r="AV3" s="205"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="141"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="142"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
-      <c r="I4" s="143"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="199" t="s">
+      <c r="B4" s="149"/>
+      <c r="C4" s="149"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="149"/>
+      <c r="F4" s="203"/>
+      <c r="G4" s="148"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="204"/>
+      <c r="K4" s="154" t="s">
         <v>115</v>
       </c>
-      <c r="L4" s="199"/>
-      <c r="M4" s="211"/>
-      <c r="N4" s="198" t="s">
+      <c r="L4" s="154"/>
+      <c r="M4" s="155"/>
+      <c r="N4" s="163" t="s">
         <v>116</v>
       </c>
-      <c r="O4" s="199"/>
-      <c r="P4" s="199"/>
-      <c r="Q4" s="199"/>
-      <c r="R4" s="199"/>
-      <c r="S4" s="200"/>
+      <c r="O4" s="154"/>
+      <c r="P4" s="154"/>
+      <c r="Q4" s="154"/>
+      <c r="R4" s="154"/>
+      <c r="S4" s="164"/>
       <c r="T4" s="187" t="s">
         <v>123</v>
       </c>
-      <c r="U4" s="190" t="s">
+      <c r="U4" s="188" t="s">
         <v>124</v>
       </c>
-      <c r="V4" s="193" t="s">
+      <c r="V4" s="158" t="s">
         <v>125</v>
       </c>
-      <c r="W4" s="172" t="s">
+      <c r="W4" s="171" t="s">
         <v>128</v>
       </c>
-      <c r="X4" s="172" t="s">
+      <c r="X4" s="171" t="s">
         <v>129</v>
       </c>
-      <c r="Y4" s="174" t="s">
+      <c r="Y4" s="173" t="s">
         <v>130</v>
       </c>
-      <c r="Z4" s="176" t="s">
+      <c r="Z4" s="175" t="s">
         <v>133</v>
       </c>
-      <c r="AA4" s="178" t="s">
+      <c r="AA4" s="177" t="s">
         <v>134</v>
       </c>
-      <c r="AB4" s="178" t="s">
+      <c r="AB4" s="177" t="s">
         <v>136</v>
       </c>
-      <c r="AC4" s="146" t="s">
+      <c r="AC4" s="179" t="s">
         <v>153</v>
       </c>
-      <c r="AD4" s="146" t="s">
+      <c r="AD4" s="179" t="s">
         <v>150</v>
       </c>
-      <c r="AE4" s="146" t="s">
+      <c r="AE4" s="179" t="s">
         <v>151</v>
       </c>
-      <c r="AF4" s="146" t="s">
+      <c r="AF4" s="179" t="s">
         <v>121</v>
       </c>
-      <c r="AG4" s="139"/>
-      <c r="AH4" s="140"/>
-      <c r="AI4" s="158" t="s">
+      <c r="AG4" s="201"/>
+      <c r="AH4" s="202"/>
+      <c r="AI4" s="191" t="s">
         <v>138</v>
       </c>
-      <c r="AJ4" s="154" t="s">
+      <c r="AJ4" s="193" t="s">
         <v>139</v>
       </c>
-      <c r="AK4" s="156" t="s">
+      <c r="AK4" s="197" t="s">
         <v>142</v>
       </c>
-      <c r="AL4" s="158" t="s">
+      <c r="AL4" s="191" t="s">
         <v>175</v>
       </c>
-      <c r="AM4" s="160" t="s">
+      <c r="AM4" s="189" t="s">
         <v>178</v>
       </c>
-      <c r="AN4" s="156" t="s">
+      <c r="AN4" s="197" t="s">
         <v>143</v>
       </c>
-      <c r="AO4" s="158" t="s">
+      <c r="AO4" s="191" t="s">
         <v>176</v>
       </c>
-      <c r="AP4" s="160" t="s">
+      <c r="AP4" s="189" t="s">
         <v>179</v>
       </c>
-      <c r="AQ4" s="152" t="s">
+      <c r="AQ4" s="210" t="s">
         <v>144</v>
       </c>
-      <c r="AR4" s="158" t="s">
+      <c r="AR4" s="191" t="s">
         <v>177</v>
       </c>
-      <c r="AS4" s="160" t="s">
+      <c r="AS4" s="189" t="s">
         <v>181</v>
       </c>
-      <c r="AT4" s="152" t="s">
+      <c r="AT4" s="210" t="s">
         <v>146</v>
       </c>
-      <c r="AU4" s="154" t="s">
+      <c r="AU4" s="193" t="s">
         <v>147</v>
       </c>
-      <c r="AV4" s="145"/>
+      <c r="AV4" s="205"/>
     </row>
     <row r="5" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="203" t="s">
+      <c r="A5" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="141"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="204" t="s">
+      <c r="B5" s="149"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="206" t="s">
+      <c r="G5" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="143" t="s">
+      <c r="H5" s="148" t="s">
         <v>107</v>
       </c>
-      <c r="I5" s="143"/>
-      <c r="J5" s="201" t="s">
+      <c r="I5" s="148"/>
+      <c r="J5" s="139" t="s">
         <v>111</v>
       </c>
-      <c r="K5" s="191" t="s">
+      <c r="K5" s="141" t="s">
         <v>112</v>
       </c>
-      <c r="L5" s="191" t="s">
+      <c r="L5" s="141" t="s">
         <v>113</v>
       </c>
-      <c r="M5" s="209" t="s">
+      <c r="M5" s="152" t="s">
         <v>114</v>
       </c>
-      <c r="N5" s="188" t="s">
+      <c r="N5" s="156" t="s">
         <v>117</v>
       </c>
-      <c r="O5" s="191" t="s">
+      <c r="O5" s="141" t="s">
         <v>118</v>
       </c>
-      <c r="P5" s="191" t="s">
+      <c r="P5" s="141" t="s">
         <v>119</v>
       </c>
-      <c r="Q5" s="191" t="s">
+      <c r="Q5" s="141" t="s">
         <v>120</v>
       </c>
-      <c r="R5" s="191" t="s">
+      <c r="R5" s="141" t="s">
         <v>122</v>
       </c>
-      <c r="S5" s="196" t="s">
+      <c r="S5" s="161" t="s">
         <v>121</v>
       </c>
-      <c r="T5" s="188"/>
-      <c r="U5" s="191"/>
-      <c r="V5" s="194"/>
-      <c r="W5" s="172"/>
-      <c r="X5" s="172"/>
-      <c r="Y5" s="174"/>
-      <c r="Z5" s="176"/>
-      <c r="AA5" s="178"/>
-      <c r="AB5" s="178"/>
-      <c r="AC5" s="146"/>
-      <c r="AD5" s="146"/>
-      <c r="AE5" s="146"/>
-      <c r="AF5" s="146"/>
-      <c r="AG5" s="139"/>
-      <c r="AH5" s="140"/>
-      <c r="AI5" s="158"/>
-      <c r="AJ5" s="154"/>
-      <c r="AK5" s="156"/>
-      <c r="AL5" s="158"/>
-      <c r="AM5" s="160"/>
-      <c r="AN5" s="156"/>
-      <c r="AO5" s="158"/>
-      <c r="AP5" s="160"/>
-      <c r="AQ5" s="152"/>
-      <c r="AR5" s="158"/>
-      <c r="AS5" s="160"/>
-      <c r="AT5" s="152"/>
-      <c r="AU5" s="154"/>
-      <c r="AV5" s="145"/>
+      <c r="T5" s="156"/>
+      <c r="U5" s="141"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="171"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="173"/>
+      <c r="Z5" s="175"/>
+      <c r="AA5" s="177"/>
+      <c r="AB5" s="177"/>
+      <c r="AC5" s="179"/>
+      <c r="AD5" s="179"/>
+      <c r="AE5" s="179"/>
+      <c r="AF5" s="179"/>
+      <c r="AG5" s="201"/>
+      <c r="AH5" s="202"/>
+      <c r="AI5" s="191"/>
+      <c r="AJ5" s="193"/>
+      <c r="AK5" s="197"/>
+      <c r="AL5" s="191"/>
+      <c r="AM5" s="189"/>
+      <c r="AN5" s="197"/>
+      <c r="AO5" s="191"/>
+      <c r="AP5" s="189"/>
+      <c r="AQ5" s="210"/>
+      <c r="AR5" s="191"/>
+      <c r="AS5" s="189"/>
+      <c r="AT5" s="210"/>
+      <c r="AU5" s="193"/>
+      <c r="AV5" s="205"/>
     </row>
     <row r="6" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="203"/>
-      <c r="B6" s="141"/>
-      <c r="C6" s="141"/>
-      <c r="D6" s="141"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="204"/>
-      <c r="G6" s="206"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="143"/>
-      <c r="J6" s="201"/>
-      <c r="K6" s="191"/>
-      <c r="L6" s="191"/>
-      <c r="M6" s="209"/>
-      <c r="N6" s="188"/>
-      <c r="O6" s="191"/>
-      <c r="P6" s="191"/>
-      <c r="Q6" s="191"/>
-      <c r="R6" s="191"/>
-      <c r="S6" s="196"/>
-      <c r="T6" s="188"/>
-      <c r="U6" s="191"/>
-      <c r="V6" s="194"/>
-      <c r="W6" s="172"/>
-      <c r="X6" s="172"/>
-      <c r="Y6" s="174"/>
-      <c r="Z6" s="176"/>
-      <c r="AA6" s="178"/>
-      <c r="AB6" s="178"/>
-      <c r="AC6" s="146"/>
-      <c r="AD6" s="146"/>
-      <c r="AE6" s="146"/>
-      <c r="AF6" s="146"/>
-      <c r="AG6" s="139"/>
-      <c r="AH6" s="140"/>
-      <c r="AI6" s="158"/>
-      <c r="AJ6" s="154"/>
-      <c r="AK6" s="156"/>
-      <c r="AL6" s="158"/>
-      <c r="AM6" s="160"/>
-      <c r="AN6" s="156"/>
-      <c r="AO6" s="158"/>
-      <c r="AP6" s="160"/>
-      <c r="AQ6" s="152"/>
-      <c r="AR6" s="158"/>
-      <c r="AS6" s="160"/>
-      <c r="AT6" s="152"/>
-      <c r="AU6" s="154"/>
-      <c r="AV6" s="145"/>
+      <c r="A6" s="143"/>
+      <c r="B6" s="149"/>
+      <c r="C6" s="149"/>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="144"/>
+      <c r="G6" s="146"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="139"/>
+      <c r="K6" s="141"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="152"/>
+      <c r="N6" s="156"/>
+      <c r="O6" s="141"/>
+      <c r="P6" s="141"/>
+      <c r="Q6" s="141"/>
+      <c r="R6" s="141"/>
+      <c r="S6" s="161"/>
+      <c r="T6" s="156"/>
+      <c r="U6" s="141"/>
+      <c r="V6" s="159"/>
+      <c r="W6" s="171"/>
+      <c r="X6" s="171"/>
+      <c r="Y6" s="173"/>
+      <c r="Z6" s="175"/>
+      <c r="AA6" s="177"/>
+      <c r="AB6" s="177"/>
+      <c r="AC6" s="179"/>
+      <c r="AD6" s="179"/>
+      <c r="AE6" s="179"/>
+      <c r="AF6" s="179"/>
+      <c r="AG6" s="201"/>
+      <c r="AH6" s="202"/>
+      <c r="AI6" s="191"/>
+      <c r="AJ6" s="193"/>
+      <c r="AK6" s="197"/>
+      <c r="AL6" s="191"/>
+      <c r="AM6" s="189"/>
+      <c r="AN6" s="197"/>
+      <c r="AO6" s="191"/>
+      <c r="AP6" s="189"/>
+      <c r="AQ6" s="210"/>
+      <c r="AR6" s="191"/>
+      <c r="AS6" s="189"/>
+      <c r="AT6" s="210"/>
+      <c r="AU6" s="193"/>
+      <c r="AV6" s="205"/>
     </row>
     <row r="7" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="203"/>
-      <c r="B7" s="141"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="204"/>
-      <c r="G7" s="206"/>
-      <c r="H7" s="143"/>
-      <c r="I7" s="143"/>
-      <c r="J7" s="201"/>
-      <c r="K7" s="191"/>
-      <c r="L7" s="191"/>
-      <c r="M7" s="209"/>
-      <c r="N7" s="188"/>
-      <c r="O7" s="191"/>
-      <c r="P7" s="191"/>
-      <c r="Q7" s="191"/>
-      <c r="R7" s="191"/>
-      <c r="S7" s="196"/>
-      <c r="T7" s="188"/>
-      <c r="U7" s="191"/>
-      <c r="V7" s="194"/>
-      <c r="W7" s="172"/>
-      <c r="X7" s="172"/>
-      <c r="Y7" s="174"/>
-      <c r="Z7" s="176"/>
-      <c r="AA7" s="178"/>
-      <c r="AB7" s="178"/>
-      <c r="AC7" s="146"/>
-      <c r="AD7" s="146"/>
-      <c r="AE7" s="146"/>
-      <c r="AF7" s="146"/>
-      <c r="AG7" s="139"/>
-      <c r="AH7" s="140"/>
-      <c r="AI7" s="158"/>
-      <c r="AJ7" s="154"/>
-      <c r="AK7" s="156"/>
-      <c r="AL7" s="158"/>
-      <c r="AM7" s="160"/>
-      <c r="AN7" s="156"/>
-      <c r="AO7" s="158"/>
-      <c r="AP7" s="160"/>
-      <c r="AQ7" s="152"/>
-      <c r="AR7" s="158"/>
-      <c r="AS7" s="160"/>
-      <c r="AT7" s="152"/>
-      <c r="AU7" s="154"/>
-      <c r="AV7" s="145"/>
+      <c r="A7" s="143"/>
+      <c r="B7" s="149"/>
+      <c r="C7" s="149"/>
+      <c r="D7" s="149"/>
+      <c r="E7" s="149"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="146"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="152"/>
+      <c r="N7" s="156"/>
+      <c r="O7" s="141"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="S7" s="161"/>
+      <c r="T7" s="156"/>
+      <c r="U7" s="141"/>
+      <c r="V7" s="159"/>
+      <c r="W7" s="171"/>
+      <c r="X7" s="171"/>
+      <c r="Y7" s="173"/>
+      <c r="Z7" s="175"/>
+      <c r="AA7" s="177"/>
+      <c r="AB7" s="177"/>
+      <c r="AC7" s="179"/>
+      <c r="AD7" s="179"/>
+      <c r="AE7" s="179"/>
+      <c r="AF7" s="179"/>
+      <c r="AG7" s="201"/>
+      <c r="AH7" s="202"/>
+      <c r="AI7" s="191"/>
+      <c r="AJ7" s="193"/>
+      <c r="AK7" s="197"/>
+      <c r="AL7" s="191"/>
+      <c r="AM7" s="189"/>
+      <c r="AN7" s="197"/>
+      <c r="AO7" s="191"/>
+      <c r="AP7" s="189"/>
+      <c r="AQ7" s="210"/>
+      <c r="AR7" s="191"/>
+      <c r="AS7" s="189"/>
+      <c r="AT7" s="210"/>
+      <c r="AU7" s="193"/>
+      <c r="AV7" s="205"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A8" s="203"/>
-      <c r="B8" s="141"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="141"/>
-      <c r="F8" s="204"/>
-      <c r="G8" s="206"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="143"/>
-      <c r="J8" s="201"/>
-      <c r="K8" s="191"/>
-      <c r="L8" s="191"/>
-      <c r="M8" s="209"/>
-      <c r="N8" s="188"/>
-      <c r="O8" s="191"/>
-      <c r="P8" s="191"/>
-      <c r="Q8" s="191"/>
-      <c r="R8" s="191"/>
-      <c r="S8" s="196"/>
-      <c r="T8" s="188"/>
-      <c r="U8" s="191"/>
-      <c r="V8" s="194"/>
-      <c r="W8" s="172"/>
-      <c r="X8" s="172"/>
-      <c r="Y8" s="174"/>
-      <c r="Z8" s="176"/>
-      <c r="AA8" s="178"/>
-      <c r="AB8" s="178"/>
-      <c r="AC8" s="146"/>
-      <c r="AD8" s="146"/>
-      <c r="AE8" s="146"/>
-      <c r="AF8" s="146"/>
-      <c r="AG8" s="139"/>
-      <c r="AH8" s="140"/>
-      <c r="AI8" s="158"/>
-      <c r="AJ8" s="154"/>
-      <c r="AK8" s="156"/>
-      <c r="AL8" s="158"/>
-      <c r="AM8" s="160"/>
-      <c r="AN8" s="156"/>
-      <c r="AO8" s="158"/>
-      <c r="AP8" s="160"/>
-      <c r="AQ8" s="152"/>
-      <c r="AR8" s="158"/>
-      <c r="AS8" s="160"/>
-      <c r="AT8" s="152"/>
-      <c r="AU8" s="154"/>
-      <c r="AV8" s="145"/>
+      <c r="A8" s="143"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="149"/>
+      <c r="E8" s="149"/>
+      <c r="F8" s="144"/>
+      <c r="G8" s="146"/>
+      <c r="H8" s="148"/>
+      <c r="I8" s="148"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="141"/>
+      <c r="M8" s="152"/>
+      <c r="N8" s="156"/>
+      <c r="O8" s="141"/>
+      <c r="P8" s="141"/>
+      <c r="Q8" s="141"/>
+      <c r="R8" s="141"/>
+      <c r="S8" s="161"/>
+      <c r="T8" s="156"/>
+      <c r="U8" s="141"/>
+      <c r="V8" s="159"/>
+      <c r="W8" s="171"/>
+      <c r="X8" s="171"/>
+      <c r="Y8" s="173"/>
+      <c r="Z8" s="175"/>
+      <c r="AA8" s="177"/>
+      <c r="AB8" s="177"/>
+      <c r="AC8" s="179"/>
+      <c r="AD8" s="179"/>
+      <c r="AE8" s="179"/>
+      <c r="AF8" s="179"/>
+      <c r="AG8" s="201"/>
+      <c r="AH8" s="202"/>
+      <c r="AI8" s="191"/>
+      <c r="AJ8" s="193"/>
+      <c r="AK8" s="197"/>
+      <c r="AL8" s="191"/>
+      <c r="AM8" s="189"/>
+      <c r="AN8" s="197"/>
+      <c r="AO8" s="191"/>
+      <c r="AP8" s="189"/>
+      <c r="AQ8" s="210"/>
+      <c r="AR8" s="191"/>
+      <c r="AS8" s="189"/>
+      <c r="AT8" s="210"/>
+      <c r="AU8" s="193"/>
+      <c r="AV8" s="205"/>
     </row>
     <row r="9" spans="1:48" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="203"/>
+      <c r="A9" s="143"/>
       <c r="B9" s="17" t="s">
         <v>1</v>
       </c>
@@ -4812,56 +4812,56 @@
       <c r="E9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="205"/>
-      <c r="G9" s="207"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="147"/>
       <c r="H9" s="19" t="s">
         <v>105</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="J9" s="202"/>
-      <c r="K9" s="192"/>
-      <c r="L9" s="192"/>
-      <c r="M9" s="210"/>
-      <c r="N9" s="189"/>
-      <c r="O9" s="192"/>
-      <c r="P9" s="192"/>
-      <c r="Q9" s="192"/>
-      <c r="R9" s="192"/>
-      <c r="S9" s="197"/>
-      <c r="T9" s="189"/>
-      <c r="U9" s="192"/>
-      <c r="V9" s="195"/>
-      <c r="W9" s="173"/>
-      <c r="X9" s="173"/>
-      <c r="Y9" s="175"/>
-      <c r="Z9" s="177"/>
-      <c r="AA9" s="179"/>
-      <c r="AB9" s="179"/>
-      <c r="AC9" s="147"/>
-      <c r="AD9" s="147"/>
-      <c r="AE9" s="147"/>
-      <c r="AF9" s="147"/>
+      <c r="J9" s="140"/>
+      <c r="K9" s="142"/>
+      <c r="L9" s="142"/>
+      <c r="M9" s="153"/>
+      <c r="N9" s="157"/>
+      <c r="O9" s="142"/>
+      <c r="P9" s="142"/>
+      <c r="Q9" s="142"/>
+      <c r="R9" s="142"/>
+      <c r="S9" s="162"/>
+      <c r="T9" s="157"/>
+      <c r="U9" s="142"/>
+      <c r="V9" s="160"/>
+      <c r="W9" s="172"/>
+      <c r="X9" s="172"/>
+      <c r="Y9" s="174"/>
+      <c r="Z9" s="176"/>
+      <c r="AA9" s="178"/>
+      <c r="AB9" s="178"/>
+      <c r="AC9" s="180"/>
+      <c r="AD9" s="180"/>
+      <c r="AE9" s="180"/>
+      <c r="AF9" s="180"/>
       <c r="AG9" s="55" t="s">
         <v>137</v>
       </c>
       <c r="AH9" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="AI9" s="159"/>
-      <c r="AJ9" s="155"/>
-      <c r="AK9" s="157"/>
-      <c r="AL9" s="159"/>
-      <c r="AM9" s="161"/>
-      <c r="AN9" s="157"/>
-      <c r="AO9" s="159"/>
-      <c r="AP9" s="161"/>
-      <c r="AQ9" s="153"/>
-      <c r="AR9" s="159"/>
-      <c r="AS9" s="161"/>
-      <c r="AT9" s="153"/>
-      <c r="AU9" s="155"/>
+      <c r="AI9" s="192"/>
+      <c r="AJ9" s="194"/>
+      <c r="AK9" s="198"/>
+      <c r="AL9" s="192"/>
+      <c r="AM9" s="190"/>
+      <c r="AN9" s="198"/>
+      <c r="AO9" s="192"/>
+      <c r="AP9" s="190"/>
+      <c r="AQ9" s="211"/>
+      <c r="AR9" s="192"/>
+      <c r="AS9" s="190"/>
+      <c r="AT9" s="211"/>
+      <c r="AU9" s="194"/>
       <c r="AV9" s="20" t="s">
         <v>148</v>
       </c>
@@ -8853,6 +8853,52 @@
     <row r="110" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="AG4:AG8"/>
+    <mergeCell ref="AH4:AH8"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="AV2:AV8"/>
+    <mergeCell ref="AE4:AE9"/>
+    <mergeCell ref="AC4:AC9"/>
+    <mergeCell ref="AI2:AU2"/>
+    <mergeCell ref="AT3:AU3"/>
+    <mergeCell ref="AT4:AT9"/>
+    <mergeCell ref="AU4:AU9"/>
+    <mergeCell ref="AN4:AN9"/>
+    <mergeCell ref="AO4:AO9"/>
+    <mergeCell ref="AP4:AP9"/>
+    <mergeCell ref="AQ4:AQ9"/>
+    <mergeCell ref="AR4:AR9"/>
+    <mergeCell ref="AS4:AS9"/>
+    <mergeCell ref="AI4:AI9"/>
+    <mergeCell ref="AJ4:AJ9"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="AK4:AK9"/>
+    <mergeCell ref="AL4:AL9"/>
+    <mergeCell ref="AM4:AM9"/>
+    <mergeCell ref="AK3:AS3"/>
+    <mergeCell ref="K2:V2"/>
+    <mergeCell ref="W2:AH2"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="W4:W9"/>
+    <mergeCell ref="X4:X9"/>
+    <mergeCell ref="Y4:Y9"/>
+    <mergeCell ref="Z4:Z9"/>
+    <mergeCell ref="AA4:AA9"/>
+    <mergeCell ref="AB4:AB9"/>
+    <mergeCell ref="AD4:AD9"/>
+    <mergeCell ref="AF4:AF9"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="Z3:AF3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="T4:T9"/>
+    <mergeCell ref="U4:U9"/>
+    <mergeCell ref="P5:P9"/>
+    <mergeCell ref="V4:V9"/>
+    <mergeCell ref="Q5:Q9"/>
+    <mergeCell ref="R5:R9"/>
+    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="N4:S4"/>
     <mergeCell ref="J5:J9"/>
     <mergeCell ref="K5:K9"/>
     <mergeCell ref="L5:L9"/>
@@ -8869,52 +8915,6 @@
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="N5:N9"/>
     <mergeCell ref="O5:O9"/>
-    <mergeCell ref="P5:P9"/>
-    <mergeCell ref="V4:V9"/>
-    <mergeCell ref="Q5:Q9"/>
-    <mergeCell ref="R5:R9"/>
-    <mergeCell ref="S5:S9"/>
-    <mergeCell ref="N4:S4"/>
-    <mergeCell ref="K2:V2"/>
-    <mergeCell ref="W2:AH2"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="W4:W9"/>
-    <mergeCell ref="X4:X9"/>
-    <mergeCell ref="Y4:Y9"/>
-    <mergeCell ref="Z4:Z9"/>
-    <mergeCell ref="AA4:AA9"/>
-    <mergeCell ref="AB4:AB9"/>
-    <mergeCell ref="AD4:AD9"/>
-    <mergeCell ref="AF4:AF9"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="Z3:AF3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="T4:T9"/>
-    <mergeCell ref="U4:U9"/>
-    <mergeCell ref="AS4:AS9"/>
-    <mergeCell ref="AI4:AI9"/>
-    <mergeCell ref="AJ4:AJ9"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="AK4:AK9"/>
-    <mergeCell ref="AL4:AL9"/>
-    <mergeCell ref="AM4:AM9"/>
-    <mergeCell ref="AK3:AS3"/>
-    <mergeCell ref="AG4:AG8"/>
-    <mergeCell ref="AH4:AH8"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="AV2:AV8"/>
-    <mergeCell ref="AE4:AE9"/>
-    <mergeCell ref="AC4:AC9"/>
-    <mergeCell ref="AI2:AU2"/>
-    <mergeCell ref="AT3:AU3"/>
-    <mergeCell ref="AT4:AT9"/>
-    <mergeCell ref="AU4:AU9"/>
-    <mergeCell ref="AN4:AN9"/>
-    <mergeCell ref="AO4:AO9"/>
-    <mergeCell ref="AP4:AP9"/>
-    <mergeCell ref="AQ4:AQ9"/>
-    <mergeCell ref="AR4:AR9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8924,7 +8924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AV84"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8940,369 +8940,369 @@
   <sheetData>
     <row r="1" spans="2:48" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="247" t="s">
         <v>310</v>
       </c>
-      <c r="C2" s="216"/>
-      <c r="D2" s="217"/>
+      <c r="C2" s="248"/>
+      <c r="D2" s="249"/>
     </row>
     <row r="3" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="218"/>
-      <c r="C3" s="219"/>
-      <c r="D3" s="220"/>
+      <c r="B3" s="250"/>
+      <c r="C3" s="251"/>
+      <c r="D3" s="252"/>
     </row>
     <row r="4" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="218"/>
-      <c r="C4" s="219"/>
-      <c r="D4" s="220"/>
+      <c r="B4" s="250"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="252"/>
     </row>
     <row r="5" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="218"/>
-      <c r="C5" s="219"/>
-      <c r="D5" s="220"/>
+      <c r="B5" s="250"/>
+      <c r="C5" s="251"/>
+      <c r="D5" s="252"/>
     </row>
     <row r="6" spans="2:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="221"/>
-      <c r="C6" s="222"/>
-      <c r="D6" s="223"/>
+      <c r="B6" s="253"/>
+      <c r="C6" s="254"/>
+      <c r="D6" s="255"/>
     </row>
     <row r="8" spans="2:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="212" t="s">
+      <c r="B9" s="244" t="s">
         <v>319</v>
       </c>
-      <c r="C9" s="213"/>
-      <c r="D9" s="213"/>
-      <c r="E9" s="213"/>
-      <c r="F9" s="214"/>
-      <c r="G9" s="257" t="s">
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="246"/>
+      <c r="G9" s="212" t="s">
         <v>131</v>
       </c>
-      <c r="H9" s="258"/>
-      <c r="I9" s="259"/>
-      <c r="J9" s="260" t="s">
+      <c r="H9" s="213"/>
+      <c r="I9" s="214"/>
+      <c r="J9" s="224" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="261"/>
-      <c r="L9" s="261"/>
-      <c r="M9" s="261"/>
-      <c r="N9" s="261"/>
-      <c r="O9" s="261"/>
-      <c r="P9" s="261"/>
-      <c r="Q9" s="261"/>
-      <c r="R9" s="261"/>
-      <c r="S9" s="261"/>
-      <c r="T9" s="261"/>
-      <c r="U9" s="261"/>
-      <c r="V9" s="261"/>
-      <c r="W9" s="261"/>
-      <c r="X9" s="261"/>
-      <c r="Y9" s="261"/>
-      <c r="Z9" s="261"/>
-      <c r="AA9" s="261"/>
-      <c r="AB9" s="261"/>
-      <c r="AC9" s="261"/>
-      <c r="AD9" s="261"/>
-      <c r="AE9" s="261"/>
-      <c r="AF9" s="261"/>
-      <c r="AG9" s="261"/>
-      <c r="AH9" s="261"/>
-      <c r="AI9" s="261"/>
-      <c r="AJ9" s="261"/>
-      <c r="AK9" s="261"/>
-      <c r="AL9" s="261"/>
-      <c r="AM9" s="261"/>
-      <c r="AN9" s="261"/>
-      <c r="AO9" s="261"/>
-      <c r="AP9" s="261"/>
-      <c r="AQ9" s="261"/>
-      <c r="AR9" s="261"/>
-      <c r="AS9" s="261"/>
-      <c r="AT9" s="261"/>
-      <c r="AU9" s="261"/>
-      <c r="AV9" s="262"/>
+      <c r="K9" s="225"/>
+      <c r="L9" s="225"/>
+      <c r="M9" s="225"/>
+      <c r="N9" s="225"/>
+      <c r="O9" s="225"/>
+      <c r="P9" s="225"/>
+      <c r="Q9" s="225"/>
+      <c r="R9" s="225"/>
+      <c r="S9" s="225"/>
+      <c r="T9" s="225"/>
+      <c r="U9" s="225"/>
+      <c r="V9" s="225"/>
+      <c r="W9" s="225"/>
+      <c r="X9" s="225"/>
+      <c r="Y9" s="225"/>
+      <c r="Z9" s="225"/>
+      <c r="AA9" s="225"/>
+      <c r="AB9" s="225"/>
+      <c r="AC9" s="225"/>
+      <c r="AD9" s="225"/>
+      <c r="AE9" s="225"/>
+      <c r="AF9" s="225"/>
+      <c r="AG9" s="225"/>
+      <c r="AH9" s="225"/>
+      <c r="AI9" s="225"/>
+      <c r="AJ9" s="225"/>
+      <c r="AK9" s="225"/>
+      <c r="AL9" s="225"/>
+      <c r="AM9" s="225"/>
+      <c r="AN9" s="225"/>
+      <c r="AO9" s="225"/>
+      <c r="AP9" s="225"/>
+      <c r="AQ9" s="225"/>
+      <c r="AR9" s="225"/>
+      <c r="AS9" s="225"/>
+      <c r="AT9" s="225"/>
+      <c r="AU9" s="225"/>
+      <c r="AV9" s="226"/>
     </row>
     <row r="10" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="137"/>
       <c r="C10" s="131"/>
-      <c r="D10" s="226"/>
-      <c r="E10" s="229"/>
-      <c r="F10" s="230"/>
-      <c r="G10" s="248" t="s">
+      <c r="D10" s="258"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="262"/>
+      <c r="G10" s="227" t="s">
         <v>128</v>
       </c>
-      <c r="H10" s="250" t="s">
+      <c r="H10" s="229" t="s">
         <v>129</v>
       </c>
-      <c r="I10" s="252" t="s">
+      <c r="I10" s="231" t="s">
         <v>130</v>
       </c>
-      <c r="J10" s="237" t="s">
+      <c r="J10" s="233" t="s">
         <v>297</v>
       </c>
-      <c r="K10" s="238"/>
-      <c r="L10" s="239"/>
-      <c r="M10" s="237" t="s">
+      <c r="K10" s="216"/>
+      <c r="L10" s="217"/>
+      <c r="M10" s="233" t="s">
         <v>298</v>
       </c>
-      <c r="N10" s="238"/>
-      <c r="O10" s="239"/>
-      <c r="P10" s="237" t="s">
+      <c r="N10" s="216"/>
+      <c r="O10" s="217"/>
+      <c r="P10" s="233" t="s">
         <v>299</v>
       </c>
-      <c r="Q10" s="238"/>
-      <c r="R10" s="239"/>
-      <c r="S10" s="237" t="s">
+      <c r="Q10" s="216"/>
+      <c r="R10" s="217"/>
+      <c r="S10" s="233" t="s">
         <v>302</v>
       </c>
-      <c r="T10" s="238"/>
-      <c r="U10" s="239"/>
-      <c r="V10" s="237" t="s">
+      <c r="T10" s="216"/>
+      <c r="U10" s="217"/>
+      <c r="V10" s="233" t="s">
         <v>150</v>
       </c>
-      <c r="W10" s="238"/>
-      <c r="X10" s="239"/>
-      <c r="Y10" s="237" t="s">
+      <c r="W10" s="216"/>
+      <c r="X10" s="217"/>
+      <c r="Y10" s="233" t="s">
         <v>151</v>
       </c>
-      <c r="Z10" s="238"/>
-      <c r="AA10" s="239"/>
-      <c r="AB10" s="237" t="s">
+      <c r="Z10" s="216"/>
+      <c r="AA10" s="217"/>
+      <c r="AB10" s="233" t="s">
         <v>312</v>
       </c>
-      <c r="AC10" s="238"/>
-      <c r="AD10" s="239"/>
-      <c r="AE10" s="237" t="s">
+      <c r="AC10" s="216"/>
+      <c r="AD10" s="217"/>
+      <c r="AE10" s="233" t="s">
         <v>313</v>
       </c>
-      <c r="AF10" s="238"/>
-      <c r="AG10" s="239"/>
-      <c r="AH10" s="237" t="s">
+      <c r="AF10" s="216"/>
+      <c r="AG10" s="217"/>
+      <c r="AH10" s="233" t="s">
         <v>314</v>
       </c>
-      <c r="AI10" s="238"/>
-      <c r="AJ10" s="239"/>
-      <c r="AK10" s="237" t="s">
+      <c r="AI10" s="216"/>
+      <c r="AJ10" s="217"/>
+      <c r="AK10" s="233" t="s">
         <v>315</v>
       </c>
-      <c r="AL10" s="238"/>
-      <c r="AM10" s="239"/>
-      <c r="AN10" s="243" t="s">
+      <c r="AL10" s="216"/>
+      <c r="AM10" s="217"/>
+      <c r="AN10" s="215" t="s">
         <v>320</v>
       </c>
-      <c r="AO10" s="238"/>
-      <c r="AP10" s="239"/>
-      <c r="AQ10" s="243" t="s">
+      <c r="AO10" s="216"/>
+      <c r="AP10" s="217"/>
+      <c r="AQ10" s="215" t="s">
         <v>308</v>
       </c>
-      <c r="AR10" s="238"/>
-      <c r="AS10" s="239"/>
-      <c r="AT10" s="243" t="s">
+      <c r="AR10" s="216"/>
+      <c r="AS10" s="217"/>
+      <c r="AT10" s="215" t="s">
         <v>321</v>
       </c>
-      <c r="AU10" s="238"/>
-      <c r="AV10" s="239"/>
+      <c r="AU10" s="216"/>
+      <c r="AV10" s="217"/>
     </row>
     <row r="11" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="138"/>
       <c r="C11" s="131"/>
-      <c r="D11" s="227"/>
-      <c r="E11" s="229"/>
-      <c r="F11" s="230"/>
-      <c r="G11" s="248"/>
-      <c r="H11" s="250"/>
-      <c r="I11" s="252"/>
-      <c r="J11" s="240"/>
-      <c r="K11" s="241"/>
-      <c r="L11" s="242"/>
-      <c r="M11" s="240"/>
-      <c r="N11" s="241"/>
-      <c r="O11" s="242"/>
-      <c r="P11" s="240"/>
-      <c r="Q11" s="241"/>
-      <c r="R11" s="242"/>
-      <c r="S11" s="240"/>
-      <c r="T11" s="241"/>
-      <c r="U11" s="242"/>
-      <c r="V11" s="240"/>
-      <c r="W11" s="241"/>
-      <c r="X11" s="242"/>
-      <c r="Y11" s="240"/>
-      <c r="Z11" s="241"/>
-      <c r="AA11" s="242"/>
-      <c r="AB11" s="240"/>
-      <c r="AC11" s="241"/>
-      <c r="AD11" s="242"/>
-      <c r="AE11" s="240"/>
-      <c r="AF11" s="241"/>
-      <c r="AG11" s="242"/>
-      <c r="AH11" s="240"/>
-      <c r="AI11" s="241"/>
-      <c r="AJ11" s="242"/>
-      <c r="AK11" s="240"/>
-      <c r="AL11" s="241"/>
-      <c r="AM11" s="242"/>
-      <c r="AN11" s="244"/>
-      <c r="AO11" s="241"/>
-      <c r="AP11" s="242"/>
-      <c r="AQ11" s="244"/>
-      <c r="AR11" s="241"/>
-      <c r="AS11" s="242"/>
-      <c r="AT11" s="244"/>
-      <c r="AU11" s="241"/>
-      <c r="AV11" s="242"/>
+      <c r="D11" s="259"/>
+      <c r="E11" s="261"/>
+      <c r="F11" s="262"/>
+      <c r="G11" s="227"/>
+      <c r="H11" s="229"/>
+      <c r="I11" s="231"/>
+      <c r="J11" s="234"/>
+      <c r="K11" s="219"/>
+      <c r="L11" s="220"/>
+      <c r="M11" s="234"/>
+      <c r="N11" s="219"/>
+      <c r="O11" s="220"/>
+      <c r="P11" s="234"/>
+      <c r="Q11" s="219"/>
+      <c r="R11" s="220"/>
+      <c r="S11" s="234"/>
+      <c r="T11" s="219"/>
+      <c r="U11" s="220"/>
+      <c r="V11" s="234"/>
+      <c r="W11" s="219"/>
+      <c r="X11" s="220"/>
+      <c r="Y11" s="234"/>
+      <c r="Z11" s="219"/>
+      <c r="AA11" s="220"/>
+      <c r="AB11" s="234"/>
+      <c r="AC11" s="219"/>
+      <c r="AD11" s="220"/>
+      <c r="AE11" s="234"/>
+      <c r="AF11" s="219"/>
+      <c r="AG11" s="220"/>
+      <c r="AH11" s="234"/>
+      <c r="AI11" s="219"/>
+      <c r="AJ11" s="220"/>
+      <c r="AK11" s="234"/>
+      <c r="AL11" s="219"/>
+      <c r="AM11" s="220"/>
+      <c r="AN11" s="218"/>
+      <c r="AO11" s="219"/>
+      <c r="AP11" s="220"/>
+      <c r="AQ11" s="218"/>
+      <c r="AR11" s="219"/>
+      <c r="AS11" s="220"/>
+      <c r="AT11" s="218"/>
+      <c r="AU11" s="219"/>
+      <c r="AV11" s="220"/>
     </row>
     <row r="12" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="224" t="s">
+      <c r="B12" s="256" t="s">
         <v>317</v>
       </c>
       <c r="C12" s="131"/>
-      <c r="D12" s="227"/>
-      <c r="E12" s="229"/>
-      <c r="F12" s="230"/>
-      <c r="G12" s="248"/>
-      <c r="H12" s="250"/>
-      <c r="I12" s="252"/>
-      <c r="J12" s="240"/>
-      <c r="K12" s="241"/>
-      <c r="L12" s="242"/>
-      <c r="M12" s="240"/>
-      <c r="N12" s="241"/>
-      <c r="O12" s="242"/>
-      <c r="P12" s="240"/>
-      <c r="Q12" s="241"/>
-      <c r="R12" s="242"/>
-      <c r="S12" s="240"/>
-      <c r="T12" s="241"/>
-      <c r="U12" s="242"/>
-      <c r="V12" s="240"/>
-      <c r="W12" s="241"/>
-      <c r="X12" s="242"/>
-      <c r="Y12" s="240"/>
-      <c r="Z12" s="241"/>
-      <c r="AA12" s="242"/>
-      <c r="AB12" s="240"/>
-      <c r="AC12" s="241"/>
-      <c r="AD12" s="242"/>
-      <c r="AE12" s="240"/>
-      <c r="AF12" s="241"/>
-      <c r="AG12" s="242"/>
-      <c r="AH12" s="240"/>
-      <c r="AI12" s="241"/>
-      <c r="AJ12" s="242"/>
-      <c r="AK12" s="240"/>
-      <c r="AL12" s="241"/>
-      <c r="AM12" s="242"/>
-      <c r="AN12" s="244"/>
-      <c r="AO12" s="241"/>
-      <c r="AP12" s="242"/>
-      <c r="AQ12" s="244"/>
-      <c r="AR12" s="241"/>
-      <c r="AS12" s="242"/>
-      <c r="AT12" s="244"/>
-      <c r="AU12" s="241"/>
-      <c r="AV12" s="242"/>
+      <c r="D12" s="259"/>
+      <c r="E12" s="261"/>
+      <c r="F12" s="262"/>
+      <c r="G12" s="227"/>
+      <c r="H12" s="229"/>
+      <c r="I12" s="231"/>
+      <c r="J12" s="234"/>
+      <c r="K12" s="219"/>
+      <c r="L12" s="220"/>
+      <c r="M12" s="234"/>
+      <c r="N12" s="219"/>
+      <c r="O12" s="220"/>
+      <c r="P12" s="234"/>
+      <c r="Q12" s="219"/>
+      <c r="R12" s="220"/>
+      <c r="S12" s="234"/>
+      <c r="T12" s="219"/>
+      <c r="U12" s="220"/>
+      <c r="V12" s="234"/>
+      <c r="W12" s="219"/>
+      <c r="X12" s="220"/>
+      <c r="Y12" s="234"/>
+      <c r="Z12" s="219"/>
+      <c r="AA12" s="220"/>
+      <c r="AB12" s="234"/>
+      <c r="AC12" s="219"/>
+      <c r="AD12" s="220"/>
+      <c r="AE12" s="234"/>
+      <c r="AF12" s="219"/>
+      <c r="AG12" s="220"/>
+      <c r="AH12" s="234"/>
+      <c r="AI12" s="219"/>
+      <c r="AJ12" s="220"/>
+      <c r="AK12" s="234"/>
+      <c r="AL12" s="219"/>
+      <c r="AM12" s="220"/>
+      <c r="AN12" s="218"/>
+      <c r="AO12" s="219"/>
+      <c r="AP12" s="220"/>
+      <c r="AQ12" s="218"/>
+      <c r="AR12" s="219"/>
+      <c r="AS12" s="220"/>
+      <c r="AT12" s="218"/>
+      <c r="AU12" s="219"/>
+      <c r="AV12" s="220"/>
     </row>
     <row r="13" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="224"/>
+      <c r="B13" s="256"/>
       <c r="C13" s="131"/>
-      <c r="D13" s="227"/>
-      <c r="E13" s="229"/>
-      <c r="F13" s="230"/>
-      <c r="G13" s="248"/>
-      <c r="H13" s="250"/>
-      <c r="I13" s="252"/>
-      <c r="J13" s="240"/>
-      <c r="K13" s="241"/>
-      <c r="L13" s="242"/>
-      <c r="M13" s="240"/>
-      <c r="N13" s="241"/>
-      <c r="O13" s="242"/>
-      <c r="P13" s="240"/>
-      <c r="Q13" s="241"/>
-      <c r="R13" s="242"/>
-      <c r="S13" s="240"/>
-      <c r="T13" s="241"/>
-      <c r="U13" s="242"/>
-      <c r="V13" s="240"/>
-      <c r="W13" s="241"/>
-      <c r="X13" s="242"/>
-      <c r="Y13" s="240"/>
-      <c r="Z13" s="241"/>
-      <c r="AA13" s="242"/>
-      <c r="AB13" s="240"/>
-      <c r="AC13" s="241"/>
-      <c r="AD13" s="242"/>
-      <c r="AE13" s="240"/>
-      <c r="AF13" s="241"/>
-      <c r="AG13" s="242"/>
-      <c r="AH13" s="240"/>
-      <c r="AI13" s="241"/>
-      <c r="AJ13" s="242"/>
-      <c r="AK13" s="240"/>
-      <c r="AL13" s="241"/>
-      <c r="AM13" s="242"/>
-      <c r="AN13" s="244"/>
-      <c r="AO13" s="241"/>
-      <c r="AP13" s="242"/>
-      <c r="AQ13" s="244"/>
-      <c r="AR13" s="241"/>
-      <c r="AS13" s="242"/>
-      <c r="AT13" s="244"/>
-      <c r="AU13" s="241"/>
-      <c r="AV13" s="242"/>
+      <c r="D13" s="259"/>
+      <c r="E13" s="261"/>
+      <c r="F13" s="262"/>
+      <c r="G13" s="227"/>
+      <c r="H13" s="229"/>
+      <c r="I13" s="231"/>
+      <c r="J13" s="234"/>
+      <c r="K13" s="219"/>
+      <c r="L13" s="220"/>
+      <c r="M13" s="234"/>
+      <c r="N13" s="219"/>
+      <c r="O13" s="220"/>
+      <c r="P13" s="234"/>
+      <c r="Q13" s="219"/>
+      <c r="R13" s="220"/>
+      <c r="S13" s="234"/>
+      <c r="T13" s="219"/>
+      <c r="U13" s="220"/>
+      <c r="V13" s="234"/>
+      <c r="W13" s="219"/>
+      <c r="X13" s="220"/>
+      <c r="Y13" s="234"/>
+      <c r="Z13" s="219"/>
+      <c r="AA13" s="220"/>
+      <c r="AB13" s="234"/>
+      <c r="AC13" s="219"/>
+      <c r="AD13" s="220"/>
+      <c r="AE13" s="234"/>
+      <c r="AF13" s="219"/>
+      <c r="AG13" s="220"/>
+      <c r="AH13" s="234"/>
+      <c r="AI13" s="219"/>
+      <c r="AJ13" s="220"/>
+      <c r="AK13" s="234"/>
+      <c r="AL13" s="219"/>
+      <c r="AM13" s="220"/>
+      <c r="AN13" s="218"/>
+      <c r="AO13" s="219"/>
+      <c r="AP13" s="220"/>
+      <c r="AQ13" s="218"/>
+      <c r="AR13" s="219"/>
+      <c r="AS13" s="220"/>
+      <c r="AT13" s="218"/>
+      <c r="AU13" s="219"/>
+      <c r="AV13" s="220"/>
     </row>
     <row r="14" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="224"/>
+      <c r="B14" s="256"/>
       <c r="C14" s="131"/>
-      <c r="D14" s="228"/>
-      <c r="E14" s="229"/>
-      <c r="F14" s="230"/>
-      <c r="G14" s="248"/>
-      <c r="H14" s="250"/>
-      <c r="I14" s="252"/>
-      <c r="J14" s="240"/>
-      <c r="K14" s="241"/>
-      <c r="L14" s="242"/>
-      <c r="M14" s="240"/>
-      <c r="N14" s="241"/>
-      <c r="O14" s="242"/>
-      <c r="P14" s="240"/>
-      <c r="Q14" s="241"/>
-      <c r="R14" s="242"/>
-      <c r="S14" s="240"/>
-      <c r="T14" s="241"/>
-      <c r="U14" s="242"/>
-      <c r="V14" s="240"/>
-      <c r="W14" s="241"/>
-      <c r="X14" s="242"/>
-      <c r="Y14" s="240"/>
-      <c r="Z14" s="241"/>
-      <c r="AA14" s="242"/>
-      <c r="AB14" s="240"/>
-      <c r="AC14" s="241"/>
-      <c r="AD14" s="242"/>
-      <c r="AE14" s="240"/>
-      <c r="AF14" s="241"/>
-      <c r="AG14" s="242"/>
-      <c r="AH14" s="240"/>
-      <c r="AI14" s="241"/>
-      <c r="AJ14" s="242"/>
-      <c r="AK14" s="240"/>
-      <c r="AL14" s="241"/>
-      <c r="AM14" s="242"/>
-      <c r="AN14" s="244"/>
-      <c r="AO14" s="241"/>
-      <c r="AP14" s="242"/>
-      <c r="AQ14" s="244"/>
-      <c r="AR14" s="241"/>
-      <c r="AS14" s="242"/>
-      <c r="AT14" s="244"/>
-      <c r="AU14" s="241"/>
-      <c r="AV14" s="242"/>
+      <c r="D14" s="260"/>
+      <c r="E14" s="261"/>
+      <c r="F14" s="262"/>
+      <c r="G14" s="227"/>
+      <c r="H14" s="229"/>
+      <c r="I14" s="231"/>
+      <c r="J14" s="234"/>
+      <c r="K14" s="219"/>
+      <c r="L14" s="220"/>
+      <c r="M14" s="234"/>
+      <c r="N14" s="219"/>
+      <c r="O14" s="220"/>
+      <c r="P14" s="234"/>
+      <c r="Q14" s="219"/>
+      <c r="R14" s="220"/>
+      <c r="S14" s="234"/>
+      <c r="T14" s="219"/>
+      <c r="U14" s="220"/>
+      <c r="V14" s="234"/>
+      <c r="W14" s="219"/>
+      <c r="X14" s="220"/>
+      <c r="Y14" s="234"/>
+      <c r="Z14" s="219"/>
+      <c r="AA14" s="220"/>
+      <c r="AB14" s="234"/>
+      <c r="AC14" s="219"/>
+      <c r="AD14" s="220"/>
+      <c r="AE14" s="234"/>
+      <c r="AF14" s="219"/>
+      <c r="AG14" s="220"/>
+      <c r="AH14" s="234"/>
+      <c r="AI14" s="219"/>
+      <c r="AJ14" s="220"/>
+      <c r="AK14" s="234"/>
+      <c r="AL14" s="219"/>
+      <c r="AM14" s="220"/>
+      <c r="AN14" s="218"/>
+      <c r="AO14" s="219"/>
+      <c r="AP14" s="220"/>
+      <c r="AQ14" s="218"/>
+      <c r="AR14" s="219"/>
+      <c r="AS14" s="220"/>
+      <c r="AT14" s="218"/>
+      <c r="AU14" s="219"/>
+      <c r="AV14" s="220"/>
     </row>
     <row r="15" spans="2:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="225"/>
+      <c r="B15" s="257"/>
       <c r="C15" s="132" t="s">
         <v>318</v>
       </c>
@@ -9315,9 +9315,9 @@
       <c r="F15" s="125" t="s">
         <v>296</v>
       </c>
-      <c r="G15" s="254"/>
-      <c r="H15" s="255"/>
-      <c r="I15" s="256"/>
+      <c r="G15" s="228"/>
+      <c r="H15" s="230"/>
+      <c r="I15" s="232"/>
       <c r="J15" s="106" t="s">
         <v>300</v>
       </c>
@@ -12915,13 +12915,13 @@
       <c r="AV77" s="104"/>
     </row>
     <row r="78" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G78" s="248" t="s">
+      <c r="G78" s="227" t="s">
         <v>128</v>
       </c>
-      <c r="H78" s="250" t="s">
+      <c r="H78" s="229" t="s">
         <v>129</v>
       </c>
-      <c r="I78" s="252" t="s">
+      <c r="I78" s="231" t="s">
         <v>130</v>
       </c>
       <c r="J78" s="113" t="s">
@@ -13043,301 +13043,327 @@
       </c>
     </row>
     <row r="79" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G79" s="248"/>
-      <c r="H79" s="250"/>
-      <c r="I79" s="252"/>
-      <c r="J79" s="237" t="s">
+      <c r="G79" s="227"/>
+      <c r="H79" s="229"/>
+      <c r="I79" s="231"/>
+      <c r="J79" s="233" t="s">
         <v>297</v>
       </c>
-      <c r="K79" s="238"/>
-      <c r="L79" s="239"/>
-      <c r="M79" s="237" t="s">
+      <c r="K79" s="216"/>
+      <c r="L79" s="217"/>
+      <c r="M79" s="233" t="s">
         <v>298</v>
       </c>
-      <c r="N79" s="238"/>
-      <c r="O79" s="239"/>
-      <c r="P79" s="237" t="s">
+      <c r="N79" s="216"/>
+      <c r="O79" s="217"/>
+      <c r="P79" s="233" t="s">
         <v>299</v>
       </c>
-      <c r="Q79" s="238"/>
-      <c r="R79" s="239"/>
-      <c r="S79" s="237" t="s">
+      <c r="Q79" s="216"/>
+      <c r="R79" s="217"/>
+      <c r="S79" s="233" t="s">
         <v>302</v>
       </c>
-      <c r="T79" s="238"/>
-      <c r="U79" s="239"/>
-      <c r="V79" s="237" t="s">
+      <c r="T79" s="216"/>
+      <c r="U79" s="217"/>
+      <c r="V79" s="233" t="s">
         <v>150</v>
       </c>
-      <c r="W79" s="238"/>
-      <c r="X79" s="239"/>
-      <c r="Y79" s="237" t="s">
+      <c r="W79" s="216"/>
+      <c r="X79" s="217"/>
+      <c r="Y79" s="233" t="s">
         <v>151</v>
       </c>
-      <c r="Z79" s="238"/>
-      <c r="AA79" s="239"/>
-      <c r="AB79" s="237" t="s">
+      <c r="Z79" s="216"/>
+      <c r="AA79" s="217"/>
+      <c r="AB79" s="233" t="s">
         <v>312</v>
       </c>
-      <c r="AC79" s="238"/>
-      <c r="AD79" s="239"/>
-      <c r="AE79" s="237" t="s">
+      <c r="AC79" s="216"/>
+      <c r="AD79" s="217"/>
+      <c r="AE79" s="233" t="s">
         <v>313</v>
       </c>
-      <c r="AF79" s="238"/>
-      <c r="AG79" s="239"/>
-      <c r="AH79" s="237" t="s">
+      <c r="AF79" s="216"/>
+      <c r="AG79" s="217"/>
+      <c r="AH79" s="233" t="s">
         <v>314</v>
       </c>
-      <c r="AI79" s="238"/>
-      <c r="AJ79" s="239"/>
-      <c r="AK79" s="237" t="s">
+      <c r="AI79" s="216"/>
+      <c r="AJ79" s="217"/>
+      <c r="AK79" s="233" t="s">
         <v>315</v>
       </c>
-      <c r="AL79" s="238"/>
-      <c r="AM79" s="239"/>
-      <c r="AN79" s="243" t="s">
+      <c r="AL79" s="216"/>
+      <c r="AM79" s="217"/>
+      <c r="AN79" s="215" t="s">
         <v>308</v>
       </c>
-      <c r="AO79" s="238"/>
-      <c r="AP79" s="239"/>
-      <c r="AQ79" s="243" t="s">
+      <c r="AO79" s="216"/>
+      <c r="AP79" s="217"/>
+      <c r="AQ79" s="215" t="s">
         <v>308</v>
       </c>
-      <c r="AR79" s="238"/>
-      <c r="AS79" s="239"/>
-      <c r="AT79" s="243" t="s">
+      <c r="AR79" s="216"/>
+      <c r="AS79" s="217"/>
+      <c r="AT79" s="215" t="s">
         <v>308</v>
       </c>
-      <c r="AU79" s="238"/>
-      <c r="AV79" s="239"/>
+      <c r="AU79" s="216"/>
+      <c r="AV79" s="217"/>
     </row>
     <row r="80" spans="2:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G80" s="248"/>
-      <c r="H80" s="250"/>
-      <c r="I80" s="252"/>
-      <c r="J80" s="240"/>
-      <c r="K80" s="241"/>
-      <c r="L80" s="242"/>
-      <c r="M80" s="240"/>
-      <c r="N80" s="241"/>
-      <c r="O80" s="242"/>
-      <c r="P80" s="240"/>
-      <c r="Q80" s="241"/>
-      <c r="R80" s="242"/>
-      <c r="S80" s="240"/>
-      <c r="T80" s="241"/>
-      <c r="U80" s="242"/>
-      <c r="V80" s="240"/>
-      <c r="W80" s="241"/>
-      <c r="X80" s="242"/>
-      <c r="Y80" s="240"/>
-      <c r="Z80" s="241"/>
-      <c r="AA80" s="242"/>
-      <c r="AB80" s="240"/>
-      <c r="AC80" s="241"/>
-      <c r="AD80" s="242"/>
-      <c r="AE80" s="240"/>
-      <c r="AF80" s="241"/>
-      <c r="AG80" s="242"/>
-      <c r="AH80" s="240"/>
-      <c r="AI80" s="241"/>
-      <c r="AJ80" s="242"/>
-      <c r="AK80" s="240"/>
-      <c r="AL80" s="241"/>
-      <c r="AM80" s="242"/>
-      <c r="AN80" s="244"/>
-      <c r="AO80" s="241"/>
-      <c r="AP80" s="242"/>
-      <c r="AQ80" s="244"/>
-      <c r="AR80" s="241"/>
-      <c r="AS80" s="242"/>
-      <c r="AT80" s="244"/>
-      <c r="AU80" s="241"/>
-      <c r="AV80" s="242"/>
+      <c r="G80" s="227"/>
+      <c r="H80" s="229"/>
+      <c r="I80" s="231"/>
+      <c r="J80" s="234"/>
+      <c r="K80" s="219"/>
+      <c r="L80" s="220"/>
+      <c r="M80" s="234"/>
+      <c r="N80" s="219"/>
+      <c r="O80" s="220"/>
+      <c r="P80" s="234"/>
+      <c r="Q80" s="219"/>
+      <c r="R80" s="220"/>
+      <c r="S80" s="234"/>
+      <c r="T80" s="219"/>
+      <c r="U80" s="220"/>
+      <c r="V80" s="234"/>
+      <c r="W80" s="219"/>
+      <c r="X80" s="220"/>
+      <c r="Y80" s="234"/>
+      <c r="Z80" s="219"/>
+      <c r="AA80" s="220"/>
+      <c r="AB80" s="234"/>
+      <c r="AC80" s="219"/>
+      <c r="AD80" s="220"/>
+      <c r="AE80" s="234"/>
+      <c r="AF80" s="219"/>
+      <c r="AG80" s="220"/>
+      <c r="AH80" s="234"/>
+      <c r="AI80" s="219"/>
+      <c r="AJ80" s="220"/>
+      <c r="AK80" s="234"/>
+      <c r="AL80" s="219"/>
+      <c r="AM80" s="220"/>
+      <c r="AN80" s="218"/>
+      <c r="AO80" s="219"/>
+      <c r="AP80" s="220"/>
+      <c r="AQ80" s="218"/>
+      <c r="AR80" s="219"/>
+      <c r="AS80" s="220"/>
+      <c r="AT80" s="218"/>
+      <c r="AU80" s="219"/>
+      <c r="AV80" s="220"/>
     </row>
     <row r="81" spans="7:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G81" s="248"/>
-      <c r="H81" s="250"/>
-      <c r="I81" s="252"/>
-      <c r="J81" s="240"/>
-      <c r="K81" s="241"/>
-      <c r="L81" s="242"/>
-      <c r="M81" s="240"/>
-      <c r="N81" s="241"/>
-      <c r="O81" s="242"/>
-      <c r="P81" s="240"/>
-      <c r="Q81" s="241"/>
-      <c r="R81" s="242"/>
-      <c r="S81" s="240"/>
-      <c r="T81" s="241"/>
-      <c r="U81" s="242"/>
-      <c r="V81" s="240"/>
-      <c r="W81" s="241"/>
-      <c r="X81" s="242"/>
-      <c r="Y81" s="240"/>
-      <c r="Z81" s="241"/>
-      <c r="AA81" s="242"/>
-      <c r="AB81" s="240"/>
-      <c r="AC81" s="241"/>
-      <c r="AD81" s="242"/>
-      <c r="AE81" s="240"/>
-      <c r="AF81" s="241"/>
-      <c r="AG81" s="242"/>
-      <c r="AH81" s="240"/>
-      <c r="AI81" s="241"/>
-      <c r="AJ81" s="242"/>
-      <c r="AK81" s="240"/>
-      <c r="AL81" s="241"/>
-      <c r="AM81" s="242"/>
-      <c r="AN81" s="244"/>
-      <c r="AO81" s="241"/>
-      <c r="AP81" s="242"/>
-      <c r="AQ81" s="244"/>
-      <c r="AR81" s="241"/>
-      <c r="AS81" s="242"/>
-      <c r="AT81" s="244"/>
-      <c r="AU81" s="241"/>
-      <c r="AV81" s="242"/>
+      <c r="G81" s="227"/>
+      <c r="H81" s="229"/>
+      <c r="I81" s="231"/>
+      <c r="J81" s="234"/>
+      <c r="K81" s="219"/>
+      <c r="L81" s="220"/>
+      <c r="M81" s="234"/>
+      <c r="N81" s="219"/>
+      <c r="O81" s="220"/>
+      <c r="P81" s="234"/>
+      <c r="Q81" s="219"/>
+      <c r="R81" s="220"/>
+      <c r="S81" s="234"/>
+      <c r="T81" s="219"/>
+      <c r="U81" s="220"/>
+      <c r="V81" s="234"/>
+      <c r="W81" s="219"/>
+      <c r="X81" s="220"/>
+      <c r="Y81" s="234"/>
+      <c r="Z81" s="219"/>
+      <c r="AA81" s="220"/>
+      <c r="AB81" s="234"/>
+      <c r="AC81" s="219"/>
+      <c r="AD81" s="220"/>
+      <c r="AE81" s="234"/>
+      <c r="AF81" s="219"/>
+      <c r="AG81" s="220"/>
+      <c r="AH81" s="234"/>
+      <c r="AI81" s="219"/>
+      <c r="AJ81" s="220"/>
+      <c r="AK81" s="234"/>
+      <c r="AL81" s="219"/>
+      <c r="AM81" s="220"/>
+      <c r="AN81" s="218"/>
+      <c r="AO81" s="219"/>
+      <c r="AP81" s="220"/>
+      <c r="AQ81" s="218"/>
+      <c r="AR81" s="219"/>
+      <c r="AS81" s="220"/>
+      <c r="AT81" s="218"/>
+      <c r="AU81" s="219"/>
+      <c r="AV81" s="220"/>
     </row>
     <row r="82" spans="7:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G82" s="248"/>
-      <c r="H82" s="250"/>
-      <c r="I82" s="252"/>
-      <c r="J82" s="240"/>
-      <c r="K82" s="241"/>
-      <c r="L82" s="242"/>
-      <c r="M82" s="240"/>
-      <c r="N82" s="241"/>
-      <c r="O82" s="242"/>
-      <c r="P82" s="240"/>
-      <c r="Q82" s="241"/>
-      <c r="R82" s="242"/>
-      <c r="S82" s="240"/>
-      <c r="T82" s="241"/>
-      <c r="U82" s="242"/>
-      <c r="V82" s="240"/>
-      <c r="W82" s="241"/>
-      <c r="X82" s="242"/>
-      <c r="Y82" s="240"/>
-      <c r="Z82" s="241"/>
-      <c r="AA82" s="242"/>
-      <c r="AB82" s="240"/>
-      <c r="AC82" s="241"/>
-      <c r="AD82" s="242"/>
-      <c r="AE82" s="240"/>
-      <c r="AF82" s="241"/>
-      <c r="AG82" s="242"/>
-      <c r="AH82" s="240"/>
-      <c r="AI82" s="241"/>
-      <c r="AJ82" s="242"/>
-      <c r="AK82" s="240"/>
-      <c r="AL82" s="241"/>
-      <c r="AM82" s="242"/>
-      <c r="AN82" s="244"/>
-      <c r="AO82" s="241"/>
-      <c r="AP82" s="242"/>
-      <c r="AQ82" s="244"/>
-      <c r="AR82" s="241"/>
-      <c r="AS82" s="242"/>
-      <c r="AT82" s="244"/>
-      <c r="AU82" s="241"/>
-      <c r="AV82" s="242"/>
+      <c r="G82" s="227"/>
+      <c r="H82" s="229"/>
+      <c r="I82" s="231"/>
+      <c r="J82" s="234"/>
+      <c r="K82" s="219"/>
+      <c r="L82" s="220"/>
+      <c r="M82" s="234"/>
+      <c r="N82" s="219"/>
+      <c r="O82" s="220"/>
+      <c r="P82" s="234"/>
+      <c r="Q82" s="219"/>
+      <c r="R82" s="220"/>
+      <c r="S82" s="234"/>
+      <c r="T82" s="219"/>
+      <c r="U82" s="220"/>
+      <c r="V82" s="234"/>
+      <c r="W82" s="219"/>
+      <c r="X82" s="220"/>
+      <c r="Y82" s="234"/>
+      <c r="Z82" s="219"/>
+      <c r="AA82" s="220"/>
+      <c r="AB82" s="234"/>
+      <c r="AC82" s="219"/>
+      <c r="AD82" s="220"/>
+      <c r="AE82" s="234"/>
+      <c r="AF82" s="219"/>
+      <c r="AG82" s="220"/>
+      <c r="AH82" s="234"/>
+      <c r="AI82" s="219"/>
+      <c r="AJ82" s="220"/>
+      <c r="AK82" s="234"/>
+      <c r="AL82" s="219"/>
+      <c r="AM82" s="220"/>
+      <c r="AN82" s="218"/>
+      <c r="AO82" s="219"/>
+      <c r="AP82" s="220"/>
+      <c r="AQ82" s="218"/>
+      <c r="AR82" s="219"/>
+      <c r="AS82" s="220"/>
+      <c r="AT82" s="218"/>
+      <c r="AU82" s="219"/>
+      <c r="AV82" s="220"/>
     </row>
     <row r="83" spans="7:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G83" s="249"/>
-      <c r="H83" s="251"/>
-      <c r="I83" s="253"/>
-      <c r="J83" s="240"/>
-      <c r="K83" s="241"/>
-      <c r="L83" s="242"/>
-      <c r="M83" s="240"/>
-      <c r="N83" s="241"/>
-      <c r="O83" s="242"/>
-      <c r="P83" s="240"/>
-      <c r="Q83" s="241"/>
-      <c r="R83" s="242"/>
-      <c r="S83" s="240"/>
-      <c r="T83" s="241"/>
-      <c r="U83" s="242"/>
-      <c r="V83" s="240"/>
-      <c r="W83" s="241"/>
-      <c r="X83" s="242"/>
-      <c r="Y83" s="240"/>
-      <c r="Z83" s="241"/>
-      <c r="AA83" s="242"/>
-      <c r="AB83" s="240"/>
-      <c r="AC83" s="241"/>
-      <c r="AD83" s="242"/>
-      <c r="AE83" s="240"/>
-      <c r="AF83" s="241"/>
-      <c r="AG83" s="242"/>
-      <c r="AH83" s="240"/>
-      <c r="AI83" s="241"/>
-      <c r="AJ83" s="242"/>
-      <c r="AK83" s="240"/>
-      <c r="AL83" s="241"/>
-      <c r="AM83" s="242"/>
-      <c r="AN83" s="245"/>
-      <c r="AO83" s="246"/>
-      <c r="AP83" s="247"/>
-      <c r="AQ83" s="245"/>
-      <c r="AR83" s="246"/>
-      <c r="AS83" s="247"/>
-      <c r="AT83" s="245"/>
-      <c r="AU83" s="246"/>
-      <c r="AV83" s="247"/>
+      <c r="G83" s="241"/>
+      <c r="H83" s="242"/>
+      <c r="I83" s="243"/>
+      <c r="J83" s="234"/>
+      <c r="K83" s="219"/>
+      <c r="L83" s="220"/>
+      <c r="M83" s="234"/>
+      <c r="N83" s="219"/>
+      <c r="O83" s="220"/>
+      <c r="P83" s="234"/>
+      <c r="Q83" s="219"/>
+      <c r="R83" s="220"/>
+      <c r="S83" s="234"/>
+      <c r="T83" s="219"/>
+      <c r="U83" s="220"/>
+      <c r="V83" s="234"/>
+      <c r="W83" s="219"/>
+      <c r="X83" s="220"/>
+      <c r="Y83" s="234"/>
+      <c r="Z83" s="219"/>
+      <c r="AA83" s="220"/>
+      <c r="AB83" s="234"/>
+      <c r="AC83" s="219"/>
+      <c r="AD83" s="220"/>
+      <c r="AE83" s="234"/>
+      <c r="AF83" s="219"/>
+      <c r="AG83" s="220"/>
+      <c r="AH83" s="234"/>
+      <c r="AI83" s="219"/>
+      <c r="AJ83" s="220"/>
+      <c r="AK83" s="234"/>
+      <c r="AL83" s="219"/>
+      <c r="AM83" s="220"/>
+      <c r="AN83" s="221"/>
+      <c r="AO83" s="222"/>
+      <c r="AP83" s="223"/>
+      <c r="AQ83" s="221"/>
+      <c r="AR83" s="222"/>
+      <c r="AS83" s="223"/>
+      <c r="AT83" s="221"/>
+      <c r="AU83" s="222"/>
+      <c r="AV83" s="223"/>
     </row>
     <row r="84" spans="7:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G84" s="231" t="s">
+      <c r="G84" s="235" t="s">
         <v>131</v>
       </c>
-      <c r="H84" s="232"/>
-      <c r="I84" s="233"/>
-      <c r="J84" s="234" t="s">
+      <c r="H84" s="236"/>
+      <c r="I84" s="237"/>
+      <c r="J84" s="238" t="s">
         <v>132</v>
       </c>
-      <c r="K84" s="235"/>
-      <c r="L84" s="235"/>
-      <c r="M84" s="235"/>
-      <c r="N84" s="235"/>
-      <c r="O84" s="235"/>
-      <c r="P84" s="235"/>
-      <c r="Q84" s="235"/>
-      <c r="R84" s="235"/>
-      <c r="S84" s="235"/>
-      <c r="T84" s="235"/>
-      <c r="U84" s="235"/>
-      <c r="V84" s="235"/>
-      <c r="W84" s="235"/>
-      <c r="X84" s="235"/>
-      <c r="Y84" s="235"/>
-      <c r="Z84" s="235"/>
-      <c r="AA84" s="235"/>
-      <c r="AB84" s="235"/>
-      <c r="AC84" s="235"/>
-      <c r="AD84" s="235"/>
-      <c r="AE84" s="235"/>
-      <c r="AF84" s="235"/>
-      <c r="AG84" s="235"/>
-      <c r="AH84" s="235"/>
-      <c r="AI84" s="235"/>
-      <c r="AJ84" s="235"/>
-      <c r="AK84" s="235"/>
-      <c r="AL84" s="235"/>
-      <c r="AM84" s="235"/>
-      <c r="AN84" s="235"/>
-      <c r="AO84" s="235"/>
-      <c r="AP84" s="235"/>
-      <c r="AQ84" s="235"/>
-      <c r="AR84" s="235"/>
-      <c r="AS84" s="236"/>
+      <c r="K84" s="239"/>
+      <c r="L84" s="239"/>
+      <c r="M84" s="239"/>
+      <c r="N84" s="239"/>
+      <c r="O84" s="239"/>
+      <c r="P84" s="239"/>
+      <c r="Q84" s="239"/>
+      <c r="R84" s="239"/>
+      <c r="S84" s="239"/>
+      <c r="T84" s="239"/>
+      <c r="U84" s="239"/>
+      <c r="V84" s="239"/>
+      <c r="W84" s="239"/>
+      <c r="X84" s="239"/>
+      <c r="Y84" s="239"/>
+      <c r="Z84" s="239"/>
+      <c r="AA84" s="239"/>
+      <c r="AB84" s="239"/>
+      <c r="AC84" s="239"/>
+      <c r="AD84" s="239"/>
+      <c r="AE84" s="239"/>
+      <c r="AF84" s="239"/>
+      <c r="AG84" s="239"/>
+      <c r="AH84" s="239"/>
+      <c r="AI84" s="239"/>
+      <c r="AJ84" s="239"/>
+      <c r="AK84" s="239"/>
+      <c r="AL84" s="239"/>
+      <c r="AM84" s="239"/>
+      <c r="AN84" s="239"/>
+      <c r="AO84" s="239"/>
+      <c r="AP84" s="239"/>
+      <c r="AQ84" s="239"/>
+      <c r="AR84" s="239"/>
+      <c r="AS84" s="240"/>
       <c r="AT84"/>
       <c r="AU84"/>
       <c r="AV84"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B2:D6"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="E10:E14"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="P79:R83"/>
+    <mergeCell ref="S79:U83"/>
+    <mergeCell ref="V79:X83"/>
+    <mergeCell ref="Y79:AA83"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="AQ10:AS14"/>
+    <mergeCell ref="AB10:AD14"/>
+    <mergeCell ref="AE10:AG14"/>
+    <mergeCell ref="AH10:AJ14"/>
+    <mergeCell ref="G84:I84"/>
+    <mergeCell ref="J84:AS84"/>
+    <mergeCell ref="AB79:AD83"/>
+    <mergeCell ref="AE79:AG83"/>
+    <mergeCell ref="AH79:AJ83"/>
+    <mergeCell ref="AK79:AM83"/>
+    <mergeCell ref="AQ79:AS83"/>
+    <mergeCell ref="G78:G83"/>
+    <mergeCell ref="H78:H83"/>
+    <mergeCell ref="I78:I83"/>
+    <mergeCell ref="J79:L83"/>
+    <mergeCell ref="M79:O83"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="AN10:AP14"/>
     <mergeCell ref="AN79:AP83"/>
@@ -13354,32 +13380,6 @@
     <mergeCell ref="P10:R14"/>
     <mergeCell ref="S10:U14"/>
     <mergeCell ref="V10:X14"/>
-    <mergeCell ref="AQ10:AS14"/>
-    <mergeCell ref="AB10:AD14"/>
-    <mergeCell ref="AE10:AG14"/>
-    <mergeCell ref="AH10:AJ14"/>
-    <mergeCell ref="G84:I84"/>
-    <mergeCell ref="J84:AS84"/>
-    <mergeCell ref="AB79:AD83"/>
-    <mergeCell ref="AE79:AG83"/>
-    <mergeCell ref="AH79:AJ83"/>
-    <mergeCell ref="AK79:AM83"/>
-    <mergeCell ref="AQ79:AS83"/>
-    <mergeCell ref="G78:G83"/>
-    <mergeCell ref="H78:H83"/>
-    <mergeCell ref="I78:I83"/>
-    <mergeCell ref="J79:L83"/>
-    <mergeCell ref="M79:O83"/>
-    <mergeCell ref="P79:R83"/>
-    <mergeCell ref="S79:U83"/>
-    <mergeCell ref="V79:X83"/>
-    <mergeCell ref="Y79:AA83"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:D6"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="E10:E14"/>
-    <mergeCell ref="F10:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>